<commit_message>
added Qiime blast and usearch taxonomy to sanger_mock_compare....
</commit_message>
<xml_diff>
--- a/data-for-figs/SangerMock_compare-blast_v_bowtie2_blca-qiime2/Anacapa_bowtie2_vs_blast_blca_vs_Qiime.xlsx
+++ b/data-for-figs/SangerMock_compare-blast_v_bowtie2_blca-qiime2/Anacapa_bowtie2_vs_blast_blca_vs_Qiime.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="140" yWindow="460" windowWidth="24560" windowHeight="13580" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="-2320" yWindow="940" windowWidth="29200" windowHeight="13780" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="16S" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,10 @@
     <sheet name="CO1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'16S'!$O$3:$O$172</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'18S_V4'!$C$2:$J$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'18S_V89'!$A$2:$B$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'CO1'!$A$2:$B$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'16S'!$M$3:$O$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'18S_V4'!$P$2:$R$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'18S_V89'!$M$2:$O$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'CO1'!$L$2:$N$2</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="426">
   <si>
     <t>Andrew</t>
   </si>
@@ -401,9 +401,6 @@
     <t>Firmicutes;Bacilli;Bacillales;Staphylococcaceae;Staphylococcus</t>
   </si>
   <si>
-    <t>ActinoActinoMicrococcales;Micrococcaceae;Micrococcus</t>
-  </si>
-  <si>
     <t>Firmicutes;Bacilli;Bacillales;Bacillaceae;Bacillus</t>
   </si>
   <si>
@@ -951,6 +948,372 @@
   </si>
   <si>
     <t xml:space="preserve">Table X.  CO1 Taxonomic assigment given BLAST blca, bowtie2 blca, and Qiime2 sklearn classifier with a 60% confidence cut off using CRUX unfiltered reference library </t>
+  </si>
+  <si>
+    <t>Feature ID</t>
+  </si>
+  <si>
+    <t>Taxon</t>
+  </si>
+  <si>
+    <t>Confidence</t>
+  </si>
+  <si>
+    <t>Bacteria;Firmicutes;Bacilli;Bacillales;Bacillaceae;Bacillus</t>
+  </si>
+  <si>
+    <t>Bacteria;Firmicutes;Bacilli;Bacillales;Listeriaceae;Listeria;Listeria monocytogenes</t>
+  </si>
+  <si>
+    <t>Bacteria;Bacteroidetes;Bacteroidia;Bacteroidales;Porphyromonadaceae;Porphyromonas;Porphyromonas gingivalis</t>
+  </si>
+  <si>
+    <t>Bacteria;Firmicutes;Clostridia;Clostridiales</t>
+  </si>
+  <si>
+    <t>Bacteria;Bacteroidetes;Bacteroidia;Bacteroidales;Prevotellaceae;Prevotella</t>
+  </si>
+  <si>
+    <t>Bacteria;Firmicutes;Bacilli;Lactobacillales;Streptococcaceae;Lactococcus;Lactococcus lactis</t>
+  </si>
+  <si>
+    <t>Bacteria;Bacteroidetes;Bacteroidia;Bacteroidales;Bacteroidaceae;Bacteroides</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Pseudomonadales;Pseudomonadaceae;Pseudomonas;Pseudomonas aeruginosa</t>
+  </si>
+  <si>
+    <t>Bacteria;Firmicutes;Clostridia;Clostridiales;Lachnospiraceae</t>
+  </si>
+  <si>
+    <t>Bacteria;Bacteroidetes;Bacteroidia;Bacteroidales;Prevotellaceae;Prevotella;Prevotella melaninogenica</t>
+  </si>
+  <si>
+    <t>Bacteria;Firmicutes;Bacilli;Lactobacillales;Enterococcaceae;Enterococcus</t>
+  </si>
+  <si>
+    <t>Bacteria;Bacteroidetes;Bacteroidia;Bacteroidales;Tannerellaceae;Parabacteroides</t>
+  </si>
+  <si>
+    <t>Bacteria;Actinobacteria;Actinobacteria;Micrococcales;Micrococcaceae;Micrococcus</t>
+  </si>
+  <si>
+    <t>Bacteria;Firmicutes;Bacilli;Bacillales;Staphylococcaceae;Staphylococcus</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Epsilonproteobacteria;Campylobacterales;Helicobacteraceae;Helicobacter;Helicobacter pylori</t>
+  </si>
+  <si>
+    <t>Bacteria;Firmicutes;Clostridia;Clostridiales;Clostridiaceae;Clostridium</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Morganellaceae;Proteus</t>
+  </si>
+  <si>
+    <t>Bacteria;Deinococcus-Thermus;Deinococci;Deinococcales;Deinococcaceae;Deinococcus</t>
+  </si>
+  <si>
+    <t>Bacteria;Firmicutes;Bacilli;Lactobacillales;Lactobacillaceae;Lactobacillus</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Enterobacteriaceae</t>
+  </si>
+  <si>
+    <t>Bacteria;Firmicutes;Erysipelotrichia;Erysipelotrichales;Erysipelotrichaceae</t>
+  </si>
+  <si>
+    <t>Bacteria;Firmicutes;Bacilli;Lactobacillales;Streptococcaceae;Streptococcus;Streptococcus agalactiae</t>
+  </si>
+  <si>
+    <t>Bacteria;Firmicutes;Bacilli;Lactobacillales;Streptococcaceae;Streptococcus;Streptococcus mutans</t>
+  </si>
+  <si>
+    <t>Bacteria;Firmicutes;Clostridia;Clostridiales;Ruminococcaceae</t>
+  </si>
+  <si>
+    <t>Bacteria;Actinobacteria;Actinobacteria;Actinomycetales;Actinomycetaceae;Actinomyces</t>
+  </si>
+  <si>
+    <t>Bacteria;Firmicutes;Bacilli;Lactobacillales;Streptococcaceae;Streptococcus;Streptococcus pneumoniae</t>
+  </si>
+  <si>
+    <t>Bacteria;Bacteroidetes;Bacteroidia;Bacteroidales</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Betaproteobacteria;Neisseriales;Neisseriaceae;Neisseria;Neisseria meningitidis</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Enterobacteriaceae;Escherichia;Escherichia coli</t>
+  </si>
+  <si>
+    <t>Bacteria;Bacteroidetes;Bacteroidia;Bacteroidales;Bacteroidaceae;Bacteroides;Bacteroides fragilis</t>
+  </si>
+  <si>
+    <t>Bacteria;Actinobacteria;Actinobacteria;Propionibacteriales;Propionibacteriaceae;Cutibacterium;Cutibacterium acnes</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Alphaproteobacteria;Rhodobacterales;Rhodobacteraceae;Rhodobacter;Rhodobacter sphaeroides</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Pseudomonadales;Moraxellaceae;Acinetobacter;Acinetobacter baumannii</t>
+  </si>
+  <si>
+    <t>Qiime Blast+ consensus taxonomy classifier</t>
+  </si>
+  <si>
+    <t>Bacteria;Proteobacteria;Gammaproteobacteria;Enterobacterales;Enterobacteriaceae;Enterobacter</t>
+  </si>
+  <si>
+    <t>Bacteria;Bacteroidetes;Bacteroidia;Bacteroidales;Tannerellaceae</t>
+  </si>
+  <si>
+    <t>Qiime Vsearch consensus taxonomy classifier</t>
+  </si>
+  <si>
+    <t>Arthropoda</t>
+  </si>
+  <si>
+    <t>Echinodermata;Ophiuroidea;Ophiurida</t>
+  </si>
+  <si>
+    <t>Arthropoda;Malacostraca;Decapoda</t>
+  </si>
+  <si>
+    <t>Eukaryota</t>
+  </si>
+  <si>
+    <t>Chordata;Actinopteri</t>
+  </si>
+  <si>
+    <t>Chordata;Actinopteri;Gobiiformes;Gobiidae;Coryphopterus</t>
+  </si>
+  <si>
+    <t>Arthropoda;Insecta;Diptera</t>
+  </si>
+  <si>
+    <t>Arthropoda;Malacostraca;Decapoda;Panopeidae;Panopeus</t>
+  </si>
+  <si>
+    <t>Mollusca;Gastropoda;NA;Placobranchidae;Elysia</t>
+  </si>
+  <si>
+    <t>Mollusca;Gastropoda;NA</t>
+  </si>
+  <si>
+    <t>Eukaryota;Arthropoda;Malacostraca;Decapoda</t>
+  </si>
+  <si>
+    <t>Eukaryota;Echinodermata;Ophiuroidea;Ophiurida</t>
+  </si>
+  <si>
+    <t>Eukaryota;Arthropoda;Malacostraca;Decapoda;Porcellanidae;Petrolisthes;Petrolisthes armatus</t>
+  </si>
+  <si>
+    <t>Eukaryota;Chordata;Actinopteri</t>
+  </si>
+  <si>
+    <t>Eukaryota;Arthropoda;Malacostraca;Decapoda;Panopeidae;Panopeus</t>
+  </si>
+  <si>
+    <t>Eukaryota;Arthropoda;Malacostraca;Decapoda;Panopeidae;Dyspanopeus;Dyspanopeus sayi</t>
+  </si>
+  <si>
+    <t>Eukaryota;Mollusca;Gastropoda;NA;Placobranchidae;Elysia</t>
+  </si>
+  <si>
+    <t>Eukaryota;Mollusca;Gastropoda;NA</t>
+  </si>
+  <si>
+    <t>Eukaryota;Chordata;Actinopteri;Gobiiformes;Gobiidae;Coryphopterus</t>
+  </si>
+  <si>
+    <t>Eukaryota;Arthropoda;Insecta;Diptera;Calliphoridae;Pollenia;Pollenia pediculata</t>
+  </si>
+  <si>
+    <t>Arthropoda;Insecta;Diptera;Calliphoridae;Pollenia;Pollenia pediculata</t>
+  </si>
+  <si>
+    <t>Arthropoda;Malacostraca;Decapoda;Aeglidae;Aegla</t>
+  </si>
+  <si>
+    <t>Annelida;Clitellata;Haplotaxida;Lumbricidae;Aporrectodea;Aporrectodea longa</t>
+  </si>
+  <si>
+    <t>Eukaryota;Arthropoda;Malacostraca;NA;NA;NA;Malacostraca sp. BOLD:ACQ1097</t>
+  </si>
+  <si>
+    <t>Eukaryota;Arthropoda;Malacostraca;Decapoda;Palaemonidae;Zenopontonia;Zenopontonia soror</t>
+  </si>
+  <si>
+    <t>Eukaryota;Platyhelminthes;NA;Polycladida;Pseudocerotidae</t>
+  </si>
+  <si>
+    <t>Eukaryota;Annelida;Polychaeta;Phyllodocida;Hesionidae</t>
+  </si>
+  <si>
+    <t>Eukaryota;Arthropoda;Malacostraca;Isopoda;Idoteidae;Idotea;Idotea ochotensis</t>
+  </si>
+  <si>
+    <t>Eukaryota;Annelida;Polychaeta;Phyllodocida;Polynoidae</t>
+  </si>
+  <si>
+    <t>Eukaryota;Annelida;Polychaeta;NA;NA;NA</t>
+  </si>
+  <si>
+    <t>Eukaryota;Annelida;Polychaeta</t>
+  </si>
+  <si>
+    <t>Eukaryota;Arthropoda;Malacostraca;Decapoda;Alpheidae</t>
+  </si>
+  <si>
+    <t>Eukaryota;Annelida;Polychaeta;Eunicida;Amphinomidae;Hermodice;Hermodice carunculata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBItools taxonomy classifier </t>
+  </si>
+  <si>
+    <t>Firmicutes;Clostridia;Clostridiales;Lachnospiraceae;NA;[Eubacterium] rectale</t>
+  </si>
+  <si>
+    <t>Proteobacteria;Gammaproteobacteria;Enterobacterales;Enterobacteriaceae</t>
+  </si>
+  <si>
+    <t>Proteobacteria;Gammaproteobacteria;Enterobacterales;Enterobacteriaceae;Escherichia</t>
+  </si>
+  <si>
+    <t>KU900218.1_extraction</t>
+  </si>
+  <si>
+    <t>KU900219.1_extraction</t>
+  </si>
+  <si>
+    <t>KU900220.1_extraction</t>
+  </si>
+  <si>
+    <t>KU900221.1_extraction</t>
+  </si>
+  <si>
+    <t>KU900222.1_extraction</t>
+  </si>
+  <si>
+    <t>KU900223.1_extraction</t>
+  </si>
+  <si>
+    <t>KU900224.1_extraction</t>
+  </si>
+  <si>
+    <t>KU900225.1_extraction</t>
+  </si>
+  <si>
+    <t>KU900226.1_extraction</t>
+  </si>
+  <si>
+    <t>KU900227.1_extraction</t>
+  </si>
+  <si>
+    <t>KU900228.1_extraction</t>
+  </si>
+  <si>
+    <t>KU900229.1_extraction</t>
+  </si>
+  <si>
+    <t>Eukaryota;NA;NA;Isochrysidales;Isochrysidaceae</t>
+  </si>
+  <si>
+    <t>Eukaryota;Chlorophyta;Chlorophyceae;Sphaeropleales;Scenedesmaceae</t>
+  </si>
+  <si>
+    <t>Eukaryota;NA;NA;Prymnesiales;Prymnesiaceae</t>
+  </si>
+  <si>
+    <t>Eukaryota;Eustigmatophyceae;NA;Eustigmatales;Monodopsidaceae;Nannochloropsis</t>
+  </si>
+  <si>
+    <t>Eukaryota;NA;Chrysophyceae;Chromulinales</t>
+  </si>
+  <si>
+    <t>Eukaryota;NA;Cryptophyta;Cryptomonadales;Cryptomonadaceae;Cryptomonas</t>
+  </si>
+  <si>
+    <t>Eukaryota;NA;Cryptophyta;Pyrenomonadales;Pyrenomonadaceae;Rhodomonas</t>
+  </si>
+  <si>
+    <t>Eukaryota;NA;Dinophyceae</t>
+  </si>
+  <si>
+    <t>Eukaryota;Bacillariophyta;Coscinodiscophyceae;Thalassiosirales</t>
+  </si>
+  <si>
+    <t>Eukaryota;Chlorophyta;Trebouxiophyceae</t>
+  </si>
+  <si>
+    <t>Bacillariophyta;Coscinodiscophyceae;Thalassiosirales</t>
+  </si>
+  <si>
+    <t>Chlorophyta;Trebouxiophyceae</t>
+  </si>
+  <si>
+    <t>Chlorophyta;Chlorophyceae;Sphaeropleales;Scenedesmaceae</t>
+  </si>
+  <si>
+    <t>NA;Cryptophyta;Cryptomonadales;Cryptomonadaceae;Cryptomonas</t>
+  </si>
+  <si>
+    <t>NA;Cryptophyta;Pyrenomonadales;Pyrenomonadaceae;Rhodomonas</t>
+  </si>
+  <si>
+    <t>NA;NA;Prymnesiales;Prymnesiaceae</t>
+  </si>
+  <si>
+    <t>NA;NA;Isochrysidales;Isochrysidaceae</t>
+  </si>
+  <si>
+    <t>NA;Dinophyceae;Suessiales;Symbiodiniaceae;Symbiodinium</t>
+  </si>
+  <si>
+    <t>NA;Dinophyceae</t>
+  </si>
+  <si>
+    <t>NA;Chrysophyceae;Chromulinales</t>
+  </si>
+  <si>
+    <t>Eustigmatophyceae;NA;Eustigmatales;Monodopsidaceae;Nannochloropsis</t>
+  </si>
+  <si>
+    <t>Chlorophyta;Trebouxiophyceae;Chlorellales;Chlorellaceae;Chlorella</t>
+  </si>
+  <si>
+    <t>;Cryptophyta;Cryptomonadales;Cryptomonadaceae;Cryptomonas</t>
+  </si>
+  <si>
+    <t>;Cryptophyta;Pyrenomonadales;Pyrenomonadaceae</t>
+  </si>
+  <si>
+    <t>;;Isochrysidales</t>
+  </si>
+  <si>
+    <t>;Dinophyceae;Suessiales;Symbiodiniaceae;Symbiodinium</t>
+  </si>
+  <si>
+    <t>;Dinophyceae</t>
+  </si>
+  <si>
+    <t>;Chrysophyceae;Chromulinales</t>
+  </si>
+  <si>
+    <t>Eustigmatophyceae;;Eustigmatales;Monodopsidaceae;Nannochloropsis</t>
+  </si>
+  <si>
+    <t>Chlorophyta;Chlorophyceae</t>
+  </si>
+  <si>
+    <t>;;Prymnesiales;Prymnesiaceae</t>
+  </si>
+  <si>
+    <t>;;Isochrysidales;Isochrysidaceae</t>
+  </si>
+  <si>
+    <t>;Chrysophyceae;Chromulinales;Dinobryaceae;Dinobryon</t>
   </si>
 </sst>
 </file>
@@ -1051,7 +1414,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1076,6 +1439,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1084,7 +1452,18 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1357,10 +1736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H78"/>
+  <dimension ref="A1:M79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1369,21 +1748,25 @@
     <col min="5" max="5" width="100.6640625" customWidth="1"/>
     <col min="6" max="6" width="92.83203125" customWidth="1"/>
     <col min="7" max="7" width="103.83203125" customWidth="1"/>
-    <col min="8" max="8" width="102.6640625" customWidth="1"/>
-    <col min="9" max="9" width="37.1640625" customWidth="1"/>
+    <col min="8" max="8" width="106.6640625" customWidth="1"/>
+    <col min="9" max="9" width="109" customWidth="1"/>
+    <col min="10" max="10" width="98.6640625" customWidth="1"/>
+    <col min="11" max="11" width="98" customWidth="1"/>
+    <col min="12" max="12" width="106.6640625" style="5" customWidth="1"/>
+    <col min="13" max="13" width="109" style="5" customWidth="1"/>
     <col min="15" max="15" width="68.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="B2" s="13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -1391,10 +1774,13 @@
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
-    </row>
-    <row r="3" spans="1:8" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+    </row>
+    <row r="3" spans="1:13" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>0</v>
@@ -1406,19 +1792,29 @@
         <v>2</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F3" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="H3" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="H3" s="9" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="I3" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>343</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>377</v>
+      </c>
+      <c r="M3" s="14"/>
+    </row>
+    <row r="4" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1432,7 +1828,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F4" t="s">
         <v>111</v>
@@ -1443,8 +1839,15 @@
       <c r="H4" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" t="s">
+        <v>313</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="M4"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1469,8 +1872,15 @@
       <c r="H5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" t="s">
+        <v>333</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="M5"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1495,8 +1905,15 @@
       <c r="H6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" t="s">
+        <v>333</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="M6"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1521,8 +1938,15 @@
       <c r="H7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" t="s">
+        <v>311</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="M7"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1547,8 +1971,15 @@
       <c r="H8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" t="s">
+        <v>316</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="M8"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -1573,8 +2004,15 @@
       <c r="H9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>316</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="M9"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -1599,8 +2037,15 @@
       <c r="H10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" t="s">
+        <v>313</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="M10"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -1625,8 +2070,15 @@
       <c r="H11" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" t="s">
+        <v>313</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="M11"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -1651,8 +2103,15 @@
       <c r="H12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" t="s">
+        <v>313</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="M12"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -1666,19 +2125,26 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H13" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" t="s">
+        <v>310</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="M13"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -1703,8 +2169,15 @@
       <c r="H14" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" t="s">
+        <v>330</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="M14"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
@@ -1729,8 +2202,15 @@
       <c r="H15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" t="s">
+        <v>318</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="M15"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -1753,10 +2233,17 @@
         <v>23</v>
       </c>
       <c r="H16" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+      <c r="I16" t="s">
+        <v>315</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="M16"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
@@ -1770,19 +2257,26 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H17" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" t="s">
+        <v>315</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="M17"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
@@ -1807,8 +2301,15 @@
       <c r="H18" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" t="s">
+        <v>318</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="M18"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
@@ -1833,8 +2334,15 @@
       <c r="H19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" t="s">
+        <v>318</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="M19"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
@@ -1851,16 +2359,23 @@
         <v>115</v>
       </c>
       <c r="F20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H20" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" t="s">
+        <v>315</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="M20"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
@@ -1885,8 +2400,15 @@
       <c r="H21" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" t="s">
+        <v>315</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="M21"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
@@ -1911,8 +2433,15 @@
       <c r="H22" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22" t="s">
+        <v>315</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="M22"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
@@ -1926,7 +2455,7 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F23" t="s">
         <v>116</v>
@@ -1937,8 +2466,15 @@
       <c r="H23" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" t="s">
+        <v>322</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="M23"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>33</v>
       </c>
@@ -1963,8 +2499,15 @@
       <c r="H24" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" t="s">
+        <v>327</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="M24"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
@@ -1978,19 +2521,26 @@
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H25" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+      <c r="I25" t="s">
+        <v>331</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="M25"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
@@ -2004,7 +2554,7 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F26" t="s">
         <v>111</v>
@@ -2015,8 +2565,15 @@
       <c r="H26" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26" t="s">
+        <v>313</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="M26"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
@@ -2030,7 +2587,7 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F27" t="s">
         <v>111</v>
@@ -2041,8 +2598,15 @@
       <c r="H27" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27" t="s">
+        <v>313</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="M27"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>38</v>
       </c>
@@ -2059,16 +2623,23 @@
         <v>26</v>
       </c>
       <c r="F28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H28" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28" t="s">
+        <v>318</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="M28"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>39</v>
       </c>
@@ -2093,8 +2664,15 @@
       <c r="H29" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I29" t="s">
+        <v>310</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="M29"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>41</v>
       </c>
@@ -2119,8 +2697,15 @@
       <c r="H30" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I30" t="s">
+        <v>313</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="M30"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>42</v>
       </c>
@@ -2134,7 +2719,7 @@
         <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F31" t="s">
         <v>111</v>
@@ -2145,8 +2730,15 @@
       <c r="H31" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I31" t="s">
+        <v>313</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="M31"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>43</v>
       </c>
@@ -2160,7 +2752,7 @@
         <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F32" t="s">
         <v>111</v>
@@ -2171,8 +2763,15 @@
       <c r="H32" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I32" t="s">
+        <v>313</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="M32"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>44</v>
       </c>
@@ -2186,7 +2785,7 @@
         <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F33" t="s">
         <v>111</v>
@@ -2197,8 +2796,15 @@
       <c r="H33" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I33" t="s">
+        <v>313</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="M33"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>45</v>
       </c>
@@ -2212,7 +2818,7 @@
         <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F34" t="s">
         <v>111</v>
@@ -2223,8 +2829,15 @@
       <c r="H34" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I34" t="s">
+        <v>313</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="M34"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>46</v>
       </c>
@@ -2238,7 +2851,7 @@
         <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F35" t="s">
         <v>111</v>
@@ -2249,8 +2862,15 @@
       <c r="H35" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I35" t="s">
+        <v>313</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="M35"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>47</v>
       </c>
@@ -2267,16 +2887,23 @@
         <v>119</v>
       </c>
       <c r="F36" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G36" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H36" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I36" t="s">
+        <v>324</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="M36"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>48</v>
       </c>
@@ -2290,7 +2917,7 @@
         <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F37" t="s">
         <v>120</v>
@@ -2301,8 +2928,15 @@
       <c r="H37" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I37" t="s">
+        <v>320</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="M37"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>49</v>
       </c>
@@ -2316,7 +2950,7 @@
         <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F38" t="s">
         <v>120</v>
@@ -2327,8 +2961,15 @@
       <c r="H38" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I38" t="s">
+        <v>320</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="M38"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>50</v>
       </c>
@@ -2353,8 +2994,15 @@
       <c r="H39" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I39" t="s">
+        <v>328</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="M39"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>52</v>
       </c>
@@ -2379,8 +3027,15 @@
       <c r="H40" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I40" t="s">
+        <v>334</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="M40"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>54</v>
       </c>
@@ -2405,8 +3060,15 @@
       <c r="H41" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I41" t="s">
+        <v>321</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="M41"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>56</v>
       </c>
@@ -2431,8 +3093,15 @@
       <c r="H42" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I42" t="s">
+        <v>332</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="M42"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>58</v>
       </c>
@@ -2457,8 +3126,15 @@
       <c r="H43" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I43" t="s">
+        <v>308</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="M43"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>60</v>
       </c>
@@ -2483,8 +3159,15 @@
       <c r="H44" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I44" t="s">
+        <v>309</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="M44"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>62</v>
       </c>
@@ -2509,8 +3192,15 @@
       <c r="H45" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I45" t="s">
+        <v>315</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="M45"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>64</v>
       </c>
@@ -2535,8 +3225,15 @@
       <c r="H46" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I46" t="s">
+        <v>336</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="M46"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>66</v>
       </c>
@@ -2561,8 +3258,15 @@
       <c r="H47" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I47" t="s">
+        <v>313</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="M47"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>68</v>
       </c>
@@ -2576,7 +3280,7 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F48" t="s">
         <v>69</v>
@@ -2587,8 +3291,15 @@
       <c r="H48" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I48" t="s">
+        <v>313</v>
+      </c>
+      <c r="J48" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="M48"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>70</v>
       </c>
@@ -2613,8 +3324,15 @@
       <c r="H49" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I49" t="s">
+        <v>313</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="M49"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>72</v>
       </c>
@@ -2628,19 +3346,26 @@
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F50" t="s">
         <v>112</v>
       </c>
       <c r="G50" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H50" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+        <v>378</v>
+      </c>
+      <c r="I50" t="s">
+        <v>315</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="M50"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>73</v>
       </c>
@@ -2665,8 +3390,15 @@
       <c r="H51" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I51" t="s">
+        <v>313</v>
+      </c>
+      <c r="J51" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="M51"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>75</v>
       </c>
@@ -2691,8 +3423,15 @@
       <c r="H52" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I52" t="s">
+        <v>313</v>
+      </c>
+      <c r="J52" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="M52"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>76</v>
       </c>
@@ -2717,8 +3456,15 @@
       <c r="H53" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I53" t="s">
+        <v>313</v>
+      </c>
+      <c r="J53" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="M53"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>77</v>
       </c>
@@ -2732,7 +3478,7 @@
         <v>0</v>
       </c>
       <c r="E54" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F54" t="s">
         <v>120</v>
@@ -2743,8 +3489,15 @@
       <c r="H54" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I54" t="s">
+        <v>320</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="M54"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>78</v>
       </c>
@@ -2769,8 +3522,15 @@
       <c r="H55" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I55" t="s">
+        <v>314</v>
+      </c>
+      <c r="J55" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="M55"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>80</v>
       </c>
@@ -2784,19 +3544,26 @@
         <v>0</v>
       </c>
       <c r="E56" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F56" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G56" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H56" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+      <c r="I56" t="s">
+        <v>323</v>
+      </c>
+      <c r="J56" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="M56"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>81</v>
       </c>
@@ -2810,19 +3577,26 @@
         <v>0</v>
       </c>
       <c r="E57" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F57" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G57" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H57" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+      <c r="I57" t="s">
+        <v>319</v>
+      </c>
+      <c r="J57" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="M57"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>82</v>
       </c>
@@ -2847,8 +3621,15 @@
       <c r="H58" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I58" t="s">
+        <v>312</v>
+      </c>
+      <c r="J58" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="M58"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>84</v>
       </c>
@@ -2862,19 +3643,26 @@
         <v>0</v>
       </c>
       <c r="E59" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F59" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G59" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H59" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+        <v>379</v>
+      </c>
+      <c r="I59" t="s">
+        <v>326</v>
+      </c>
+      <c r="J59" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="M59"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>85</v>
       </c>
@@ -2897,10 +3685,17 @@
         <v>86</v>
       </c>
       <c r="H60" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+        <v>380</v>
+      </c>
+      <c r="I60" t="s">
+        <v>335</v>
+      </c>
+      <c r="J60" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="M60"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>87</v>
       </c>
@@ -2914,19 +3709,26 @@
         <v>0</v>
       </c>
       <c r="E61" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F61" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G61" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H61" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="I61" t="s">
+        <v>307</v>
+      </c>
+      <c r="J61" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="M61"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>88</v>
       </c>
@@ -2951,8 +3753,15 @@
       <c r="H62" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I62" t="s">
+        <v>337</v>
+      </c>
+      <c r="J62" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="M62"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>90</v>
       </c>
@@ -2966,19 +3775,26 @@
         <v>0</v>
       </c>
       <c r="E63" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F63" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G63" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H63" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="I63" t="s">
+        <v>317</v>
+      </c>
+      <c r="J63" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="M63"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>91</v>
       </c>
@@ -2992,19 +3808,26 @@
         <v>0</v>
       </c>
       <c r="E64" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F64" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G64" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H64" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="I64" t="s">
+        <v>317</v>
+      </c>
+      <c r="J64" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="M64"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>92</v>
       </c>
@@ -3029,8 +3852,15 @@
       <c r="H65" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I65" t="s">
+        <v>329</v>
+      </c>
+      <c r="J65" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="M65"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>94</v>
       </c>
@@ -3055,8 +3885,15 @@
       <c r="H66" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I66" t="s">
+        <v>320</v>
+      </c>
+      <c r="J66" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="M66"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>95</v>
       </c>
@@ -3081,8 +3918,15 @@
       <c r="H67" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I67" t="s">
+        <v>320</v>
+      </c>
+      <c r="J67" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="M67"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>96</v>
       </c>
@@ -3107,8 +3951,15 @@
       <c r="H68" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I68" t="s">
+        <v>320</v>
+      </c>
+      <c r="J68" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="M68"/>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>98</v>
       </c>
@@ -3122,7 +3973,7 @@
         <v>0</v>
       </c>
       <c r="E69" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F69" t="s">
         <v>116</v>
@@ -3131,10 +3982,17 @@
         <v>116</v>
       </c>
       <c r="H69" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="I69" t="s">
+        <v>322</v>
+      </c>
+      <c r="J69" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="M69"/>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>99</v>
       </c>
@@ -3148,7 +4006,7 @@
         <v>0</v>
       </c>
       <c r="E70" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F70" t="s">
         <v>116</v>
@@ -3157,10 +4015,17 @@
         <v>116</v>
       </c>
       <c r="H70" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="I70" t="s">
+        <v>322</v>
+      </c>
+      <c r="J70" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="M70"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>100</v>
       </c>
@@ -3174,7 +4039,7 @@
         <v>0</v>
       </c>
       <c r="E71" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F71" t="s">
         <v>116</v>
@@ -3183,10 +4048,17 @@
         <v>116</v>
       </c>
       <c r="H71" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="I71" t="s">
+        <v>322</v>
+      </c>
+      <c r="J71" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="M71"/>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>101</v>
       </c>
@@ -3200,19 +4072,26 @@
         <v>0</v>
       </c>
       <c r="E72" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F72" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G72" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H72" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="I72" t="s">
+        <v>307</v>
+      </c>
+      <c r="J72" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="M72"/>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>102</v>
       </c>
@@ -3237,8 +4116,15 @@
       <c r="H73" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I73" t="s">
+        <v>314</v>
+      </c>
+      <c r="J73" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="M73"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>103</v>
       </c>
@@ -3263,8 +4149,15 @@
       <c r="H74" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I74" t="s">
+        <v>314</v>
+      </c>
+      <c r="J74" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="M74"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>104</v>
       </c>
@@ -3289,8 +4182,15 @@
       <c r="H75" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I75" t="s">
+        <v>338</v>
+      </c>
+      <c r="J75" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="M75"/>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>106</v>
       </c>
@@ -3315,8 +4215,15 @@
       <c r="H76" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I76" t="s">
+        <v>339</v>
+      </c>
+      <c r="J76" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="M76"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>108</v>
       </c>
@@ -3339,10 +4246,18 @@
         <v>86</v>
       </c>
       <c r="H77" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+        <v>380</v>
+      </c>
+      <c r="I77" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="J77" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="K77" s="5"/>
+      <c r="M77"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" s="11" t="s">
         <v>109</v>
       </c>
@@ -3359,14 +4274,25 @@
         <v>110</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G78" s="6" t="s">
         <v>110</v>
       </c>
       <c r="H78" s="6" t="s">
-        <v>125</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="I78" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="J78" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="K78" s="6"/>
+      <c r="M78" s="6"/>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M79"/>
     </row>
   </sheetData>
   <sortState ref="O1:O170">
@@ -3381,10 +4307,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="B13:C13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3392,248 +4318,448 @@
     <col min="1" max="1" width="13.33203125" customWidth="1"/>
     <col min="2" max="4" width="92.1640625" customWidth="1"/>
     <col min="5" max="5" width="92.83203125" customWidth="1"/>
+    <col min="6" max="6" width="103.33203125" customWidth="1"/>
+    <col min="7" max="7" width="73" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="D2" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>340</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>377</v>
+      </c>
+      <c r="P2" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>305</v>
+      </c>
+      <c r="R2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="B3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F3" t="s">
+        <v>149</v>
+      </c>
+      <c r="G3" t="s">
+        <v>403</v>
+      </c>
+      <c r="P3" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>401</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="B4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E4" t="s">
+        <v>172</v>
+      </c>
+      <c r="F4" t="s">
+        <v>172</v>
+      </c>
+      <c r="G4" t="s">
+        <v>404</v>
+      </c>
+      <c r="P4" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>402</v>
+      </c>
+      <c r="R4">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="B5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D5" t="s">
+        <v>151</v>
+      </c>
+      <c r="E5" t="s">
+        <v>151</v>
+      </c>
+      <c r="F5" t="s">
+        <v>151</v>
+      </c>
+      <c r="G5" t="s">
+        <v>151</v>
+      </c>
+      <c r="P5" t="s">
+        <v>383</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>189</v>
+      </c>
+      <c r="R5">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="B6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" t="s">
+        <v>150</v>
+      </c>
+      <c r="F6" t="s">
+        <v>150</v>
+      </c>
+      <c r="G6" t="s">
+        <v>405</v>
+      </c>
+      <c r="P6" t="s">
+        <v>384</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>394</v>
+      </c>
+      <c r="R6">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="B7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" t="s">
+        <v>153</v>
+      </c>
+      <c r="D7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E7" t="s">
+        <v>153</v>
+      </c>
+      <c r="F7" t="s">
+        <v>153</v>
+      </c>
+      <c r="G7" t="s">
+        <v>406</v>
+      </c>
+      <c r="P7" t="s">
+        <v>385</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>398</v>
+      </c>
+      <c r="R7">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="B8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C8" t="s">
+        <v>162</v>
+      </c>
+      <c r="D8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E8" t="s">
+        <v>173</v>
+      </c>
+      <c r="F8" t="s">
+        <v>173</v>
+      </c>
+      <c r="G8" t="s">
+        <v>407</v>
+      </c>
+      <c r="P8" t="s">
+        <v>386</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>399</v>
+      </c>
+      <c r="R8">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C9" t="s">
+        <v>179</v>
+      </c>
+      <c r="D9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E9" t="s">
+        <v>174</v>
+      </c>
+      <c r="F9" t="s">
+        <v>174</v>
+      </c>
+      <c r="G9" t="s">
+        <v>408</v>
+      </c>
+      <c r="P9" t="s">
+        <v>387</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>395</v>
+      </c>
+      <c r="R9">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D10" t="s">
+        <v>168</v>
+      </c>
+      <c r="E10" t="s">
+        <v>157</v>
+      </c>
+      <c r="F10" t="s">
+        <v>157</v>
+      </c>
+      <c r="G10" t="s">
+        <v>409</v>
+      </c>
+      <c r="P10" t="s">
+        <v>388</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>393</v>
+      </c>
+      <c r="R10">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="B11" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11" t="s">
+        <v>163</v>
+      </c>
+      <c r="D11" t="s">
+        <v>169</v>
+      </c>
+      <c r="E11" t="s">
+        <v>175</v>
+      </c>
+      <c r="F11" t="s">
+        <v>175</v>
+      </c>
+      <c r="G11" t="s">
+        <v>410</v>
+      </c>
+      <c r="P11" t="s">
+        <v>389</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>195</v>
+      </c>
+      <c r="R11">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="B12" t="s">
+        <v>155</v>
+      </c>
+      <c r="C12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D12" t="s">
+        <v>155</v>
+      </c>
+      <c r="E12" t="s">
+        <v>176</v>
+      </c>
+      <c r="F12" t="s">
+        <v>176</v>
+      </c>
+      <c r="G12" t="s">
+        <v>411</v>
+      </c>
+      <c r="P12" t="s">
+        <v>390</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>400</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>266</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="B3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D3" t="s">
-        <v>150</v>
-      </c>
-      <c r="E3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="B4" t="s">
-        <v>250</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C13" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="D4" t="s">
-        <v>165</v>
-      </c>
-      <c r="E4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="D13" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F13" t="s">
+        <v>177</v>
+      </c>
+      <c r="G13" t="s">
+        <v>412</v>
+      </c>
+      <c r="P13" t="s">
+        <v>391</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>397</v>
+      </c>
+      <c r="R13">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C14" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="D5" t="s">
-        <v>152</v>
-      </c>
-      <c r="E5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="B6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C6" t="s">
-        <v>160</v>
-      </c>
-      <c r="D6" t="s">
-        <v>160</v>
-      </c>
-      <c r="E6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="B7" t="s">
-        <v>154</v>
-      </c>
-      <c r="C7" t="s">
-        <v>154</v>
-      </c>
-      <c r="D7" t="s">
-        <v>166</v>
-      </c>
-      <c r="E7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="B8" t="s">
-        <v>155</v>
-      </c>
-      <c r="C8" t="s">
-        <v>163</v>
-      </c>
-      <c r="D8" t="s">
-        <v>167</v>
-      </c>
-      <c r="E8" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="B9" t="s">
-        <v>159</v>
-      </c>
-      <c r="C9" t="s">
-        <v>180</v>
-      </c>
-      <c r="D9" t="s">
-        <v>168</v>
-      </c>
-      <c r="E9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="B10" t="s">
-        <v>158</v>
-      </c>
-      <c r="C10" t="s">
-        <v>158</v>
-      </c>
-      <c r="D10" t="s">
-        <v>169</v>
-      </c>
-      <c r="E10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="B11" t="s">
-        <v>157</v>
-      </c>
-      <c r="C11" t="s">
-        <v>164</v>
-      </c>
-      <c r="D11" t="s">
-        <v>170</v>
-      </c>
-      <c r="E11" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="B12" t="s">
-        <v>156</v>
-      </c>
-      <c r="C12" t="s">
-        <v>156</v>
-      </c>
-      <c r="D12" t="s">
-        <v>156</v>
-      </c>
-      <c r="E12" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="B13" s="5" t="s">
+      <c r="D14" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="P14" t="s">
+        <v>392</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>396</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>247</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C2:J2">
-    <sortState ref="C2:J13">
-      <sortCondition ref="C1:C13"/>
+  <autoFilter ref="P2:R2">
+    <sortState ref="P3:R14">
+      <sortCondition ref="P2:P14"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3642,10 +4768,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3655,260 +4781,337 @@
     <col min="3" max="3" width="94.83203125" customWidth="1"/>
     <col min="4" max="4" width="91.6640625" customWidth="1"/>
     <col min="5" max="5" width="101.83203125" customWidth="1"/>
+    <col min="6" max="6" width="64" customWidth="1"/>
+    <col min="7" max="7" width="63" customWidth="1"/>
+    <col min="8" max="8" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="D2" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>340</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="F3" t="s">
+        <v>403</v>
+      </c>
+      <c r="G3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="F4" t="s">
+        <v>404</v>
+      </c>
+      <c r="G4" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="F5" t="s">
+        <v>414</v>
+      </c>
+      <c r="G5" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="F6" t="s">
+        <v>405</v>
+      </c>
+      <c r="G6" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="F7" t="s">
+        <v>415</v>
+      </c>
+      <c r="G7" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="F8" t="s">
+        <v>416</v>
+      </c>
+      <c r="G8" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="G9" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="F10" t="s">
+        <v>417</v>
+      </c>
+      <c r="G10" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="F11" t="s">
+        <v>418</v>
+      </c>
+      <c r="G11" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F12" t="s">
+        <v>419</v>
+      </c>
+      <c r="G12" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>266</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="D13" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="F13" t="s">
+        <v>420</v>
+      </c>
+      <c r="G13" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="C14" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D14" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="B13" s="5" t="s">
+      <c r="E14" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>247</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:B2">
-    <sortState ref="A2:C13">
-      <sortCondition ref="A1:A13"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:V36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F11" sqref="A1:H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3918,608 +5121,813 @@
     <col min="3" max="3" width="84" customWidth="1"/>
     <col min="4" max="4" width="76.83203125" customWidth="1"/>
     <col min="5" max="5" width="79.1640625" customWidth="1"/>
+    <col min="6" max="6" width="70.5" customWidth="1"/>
+    <col min="7" max="7" width="84.33203125" customWidth="1"/>
+    <col min="8" max="8" width="27.83203125" customWidth="1"/>
+    <col min="12" max="12" width="14.1640625" customWidth="1"/>
+    <col min="13" max="13" width="83.1640625" customWidth="1"/>
+    <col min="22" max="22" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="F2" s="16" t="s">
+        <v>340</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>377</v>
+      </c>
+      <c r="V2" s="15"/>
+    </row>
+    <row r="3" spans="1:22" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E3" t="s">
+        <v>199</v>
+      </c>
+      <c r="F3" t="s">
+        <v>349</v>
+      </c>
+      <c r="G3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>270</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>200</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>200</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
+        <v>236</v>
+      </c>
+      <c r="E4" t="s">
         <v>200</v>
       </c>
-      <c r="E3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="F4" t="s">
+        <v>346</v>
+      </c>
+      <c r="G4" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>271</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C5" t="s">
         <v>201</v>
       </c>
-      <c r="C4" t="s">
-        <v>201</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>237</v>
       </c>
-      <c r="E4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="E5" t="s">
+        <v>237</v>
+      </c>
+      <c r="G5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>272</v>
       </c>
-      <c r="B5" t="s">
-        <v>236</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B6" t="s">
         <v>202</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D6" t="s">
+        <v>202</v>
+      </c>
+      <c r="E6" t="s">
+        <v>202</v>
+      </c>
+      <c r="F6" t="s">
+        <v>345</v>
+      </c>
+      <c r="G6" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>273</v>
+      </c>
+      <c r="B7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C7" t="s">
+        <v>203</v>
+      </c>
+      <c r="D7" t="s">
+        <v>203</v>
+      </c>
+      <c r="E7" t="s">
+        <v>203</v>
+      </c>
+      <c r="F7" t="s">
+        <v>353</v>
+      </c>
+      <c r="G7" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>274</v>
+      </c>
+      <c r="B8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C8" t="s">
+        <v>204</v>
+      </c>
+      <c r="D8" t="s">
+        <v>204</v>
+      </c>
+      <c r="E8" t="s">
+        <v>204</v>
+      </c>
+      <c r="F8" t="s">
+        <v>348</v>
+      </c>
+      <c r="G8" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>275</v>
+      </c>
+      <c r="B9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C9" t="s">
+        <v>205</v>
+      </c>
+      <c r="D9" t="s">
+        <v>205</v>
+      </c>
+      <c r="E9" t="s">
+        <v>205</v>
+      </c>
+      <c r="F9" t="s">
+        <v>345</v>
+      </c>
+      <c r="G9" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>276</v>
+      </c>
+      <c r="B10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C10" t="s">
+        <v>206</v>
+      </c>
+      <c r="D10" t="s">
+        <v>206</v>
+      </c>
+      <c r="E10" t="s">
+        <v>206</v>
+      </c>
+      <c r="F10" t="s">
+        <v>346</v>
+      </c>
+      <c r="G10" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>277</v>
+      </c>
+      <c r="B11" t="s">
+        <v>207</v>
+      </c>
+      <c r="C11" t="s">
+        <v>207</v>
+      </c>
+      <c r="D11" t="s">
         <v>238</v>
       </c>
-      <c r="E5" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>273</v>
-      </c>
-      <c r="B6" t="s">
-        <v>203</v>
-      </c>
-      <c r="C6" t="s">
-        <v>203</v>
-      </c>
-      <c r="D6" t="s">
-        <v>203</v>
-      </c>
-      <c r="E6" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>274</v>
-      </c>
-      <c r="B7" t="s">
-        <v>204</v>
-      </c>
-      <c r="C7" t="s">
-        <v>204</v>
-      </c>
-      <c r="D7" t="s">
-        <v>204</v>
-      </c>
-      <c r="E7" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>275</v>
-      </c>
-      <c r="B8" t="s">
-        <v>205</v>
-      </c>
-      <c r="C8" t="s">
-        <v>205</v>
-      </c>
-      <c r="D8" t="s">
-        <v>205</v>
-      </c>
-      <c r="E8" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>276</v>
-      </c>
-      <c r="B9" t="s">
-        <v>206</v>
-      </c>
-      <c r="C9" t="s">
-        <v>206</v>
-      </c>
-      <c r="D9" t="s">
-        <v>206</v>
-      </c>
-      <c r="E9" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>277</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="E11" t="s">
         <v>207</v>
       </c>
-      <c r="C10" t="s">
-        <v>207</v>
-      </c>
-      <c r="D10" t="s">
-        <v>207</v>
-      </c>
-      <c r="E10" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="F11" t="s">
+        <v>348</v>
+      </c>
+      <c r="G11" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>278</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>208</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>208</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
+        <v>208</v>
+      </c>
+      <c r="E12" t="s">
+        <v>208</v>
+      </c>
+      <c r="F12" t="s">
+        <v>345</v>
+      </c>
+      <c r="G12" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>279</v>
+      </c>
+      <c r="B13" t="s">
+        <v>209</v>
+      </c>
+      <c r="C13" t="s">
+        <v>209</v>
+      </c>
+      <c r="D13" t="s">
+        <v>209</v>
+      </c>
+      <c r="E13" t="s">
+        <v>209</v>
+      </c>
+      <c r="F13" t="s">
+        <v>344</v>
+      </c>
+      <c r="G13" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>280</v>
+      </c>
+      <c r="B14" t="s">
+        <v>210</v>
+      </c>
+      <c r="C14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D14" t="s">
+        <v>210</v>
+      </c>
+      <c r="E14" t="s">
+        <v>210</v>
+      </c>
+      <c r="F14" t="s">
+        <v>351</v>
+      </c>
+      <c r="G14" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>281</v>
+      </c>
+      <c r="B15" t="s">
+        <v>211</v>
+      </c>
+      <c r="C15" t="s">
+        <v>211</v>
+      </c>
+      <c r="D15" t="s">
+        <v>211</v>
+      </c>
+      <c r="E15" t="s">
+        <v>211</v>
+      </c>
+      <c r="F15" t="s">
+        <v>346</v>
+      </c>
+      <c r="G15" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>282</v>
+      </c>
+      <c r="B16" t="s">
+        <v>212</v>
+      </c>
+      <c r="C16" t="s">
+        <v>212</v>
+      </c>
+      <c r="D16" t="s">
+        <v>212</v>
+      </c>
+      <c r="E16" t="s">
+        <v>212</v>
+      </c>
+      <c r="F16" t="s">
+        <v>364</v>
+      </c>
+      <c r="G16" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>283</v>
+      </c>
+      <c r="B17" t="s">
+        <v>213</v>
+      </c>
+      <c r="C17" t="s">
+        <v>213</v>
+      </c>
+      <c r="D17" t="s">
+        <v>213</v>
+      </c>
+      <c r="E17" t="s">
+        <v>213</v>
+      </c>
+      <c r="F17" t="s">
+        <v>346</v>
+      </c>
+      <c r="G17" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>284</v>
+      </c>
+      <c r="B18" t="s">
+        <v>214</v>
+      </c>
+      <c r="C18" t="s">
+        <v>214</v>
+      </c>
+      <c r="D18" t="s">
+        <v>214</v>
+      </c>
+      <c r="E18" t="s">
+        <v>214</v>
+      </c>
+      <c r="G18" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>285</v>
+      </c>
+      <c r="B19" t="s">
+        <v>234</v>
+      </c>
+      <c r="D19" t="s">
         <v>239</v>
       </c>
-      <c r="E11" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>279</v>
-      </c>
-      <c r="B12" t="s">
-        <v>209</v>
-      </c>
-      <c r="C12" t="s">
-        <v>209</v>
-      </c>
-      <c r="D12" t="s">
-        <v>209</v>
-      </c>
-      <c r="E12" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>280</v>
-      </c>
-      <c r="B13" t="s">
-        <v>210</v>
-      </c>
-      <c r="C13" t="s">
-        <v>210</v>
-      </c>
-      <c r="D13" t="s">
-        <v>210</v>
-      </c>
-      <c r="E13" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>281</v>
-      </c>
-      <c r="B14" t="s">
-        <v>211</v>
-      </c>
-      <c r="C14" t="s">
-        <v>211</v>
-      </c>
-      <c r="D14" t="s">
-        <v>211</v>
-      </c>
-      <c r="E14" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>282</v>
-      </c>
-      <c r="B15" t="s">
-        <v>212</v>
-      </c>
-      <c r="C15" t="s">
-        <v>212</v>
-      </c>
-      <c r="D15" t="s">
-        <v>212</v>
-      </c>
-      <c r="E15" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>283</v>
-      </c>
-      <c r="B16" t="s">
-        <v>213</v>
-      </c>
-      <c r="C16" t="s">
-        <v>213</v>
-      </c>
-      <c r="D16" t="s">
-        <v>213</v>
-      </c>
-      <c r="E16" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>284</v>
-      </c>
-      <c r="B17" t="s">
-        <v>214</v>
-      </c>
-      <c r="C17" t="s">
-        <v>214</v>
-      </c>
-      <c r="D17" t="s">
-        <v>214</v>
-      </c>
-      <c r="E17" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>285</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="G19" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>286</v>
+      </c>
+      <c r="B20" t="s">
         <v>215</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C20" t="s">
         <v>215</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D20" t="s">
+        <v>240</v>
+      </c>
+      <c r="E20" t="s">
         <v>215</v>
       </c>
-      <c r="E18" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>286</v>
-      </c>
-      <c r="B19" t="s">
-        <v>235</v>
-      </c>
-      <c r="D19" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="F20" t="s">
+        <v>346</v>
+      </c>
+      <c r="G20" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>287</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>216</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>216</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
+        <v>216</v>
+      </c>
+      <c r="E21" t="s">
+        <v>216</v>
+      </c>
+      <c r="F21" t="s">
+        <v>216</v>
+      </c>
+      <c r="G21" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>288</v>
+      </c>
+      <c r="B22" t="s">
+        <v>217</v>
+      </c>
+      <c r="C22" t="s">
+        <v>217</v>
+      </c>
+      <c r="D22" t="s">
+        <v>217</v>
+      </c>
+      <c r="E22" t="s">
+        <v>217</v>
+      </c>
+      <c r="F22" t="s">
+        <v>346</v>
+      </c>
+      <c r="G22" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>289</v>
+      </c>
+      <c r="B23" t="s">
+        <v>233</v>
+      </c>
+      <c r="C23" t="s">
+        <v>218</v>
+      </c>
+      <c r="D23" t="s">
+        <v>218</v>
+      </c>
+      <c r="E23" t="s">
+        <v>243</v>
+      </c>
+      <c r="F23" t="s">
+        <v>243</v>
+      </c>
+      <c r="G23" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>290</v>
+      </c>
+      <c r="B24" t="s">
+        <v>219</v>
+      </c>
+      <c r="C24" t="s">
+        <v>219</v>
+      </c>
+      <c r="D24" t="s">
+        <v>219</v>
+      </c>
+      <c r="E24" t="s">
+        <v>219</v>
+      </c>
+      <c r="F24" t="s">
+        <v>350</v>
+      </c>
+      <c r="G24" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>291</v>
+      </c>
+      <c r="B25" t="s">
+        <v>220</v>
+      </c>
+      <c r="C25" t="s">
+        <v>220</v>
+      </c>
+      <c r="D25" t="s">
+        <v>220</v>
+      </c>
+      <c r="E25" t="s">
+        <v>220</v>
+      </c>
+      <c r="F25" t="s">
+        <v>346</v>
+      </c>
+      <c r="G25" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>292</v>
+      </c>
+      <c r="B26" t="s">
+        <v>221</v>
+      </c>
+      <c r="C26" t="s">
+        <v>221</v>
+      </c>
+      <c r="D26" t="s">
         <v>241</v>
       </c>
-      <c r="E20" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>288</v>
-      </c>
-      <c r="B21" t="s">
-        <v>217</v>
-      </c>
-      <c r="C21" t="s">
-        <v>217</v>
-      </c>
-      <c r="D21" t="s">
-        <v>217</v>
-      </c>
-      <c r="E21" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>289</v>
-      </c>
-      <c r="B22" t="s">
-        <v>218</v>
-      </c>
-      <c r="C22" t="s">
-        <v>218</v>
-      </c>
-      <c r="D22" t="s">
-        <v>218</v>
-      </c>
-      <c r="E22" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>290</v>
-      </c>
-      <c r="B23" t="s">
-        <v>234</v>
-      </c>
-      <c r="C23" t="s">
-        <v>219</v>
-      </c>
-      <c r="D23" t="s">
-        <v>219</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="E26" t="s">
+        <v>221</v>
+      </c>
+      <c r="F26" t="s">
+        <v>365</v>
+      </c>
+      <c r="G26" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>293</v>
+      </c>
+      <c r="B27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C27" t="s">
+        <v>222</v>
+      </c>
+      <c r="D27" t="s">
+        <v>222</v>
+      </c>
+      <c r="E27" t="s">
+        <v>222</v>
+      </c>
+      <c r="F27" t="s">
+        <v>346</v>
+      </c>
+      <c r="G27" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>294</v>
+      </c>
+      <c r="B28" t="s">
+        <v>223</v>
+      </c>
+      <c r="C28" t="s">
+        <v>223</v>
+      </c>
+      <c r="D28" t="s">
+        <v>223</v>
+      </c>
+      <c r="E28" t="s">
+        <v>223</v>
+      </c>
+      <c r="F28" t="s">
+        <v>352</v>
+      </c>
+      <c r="G28" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>295</v>
+      </c>
+      <c r="B29" t="s">
+        <v>224</v>
+      </c>
+      <c r="C29" t="s">
+        <v>224</v>
+      </c>
+      <c r="D29" t="s">
+        <v>224</v>
+      </c>
+      <c r="E29" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>291</v>
-      </c>
-      <c r="B24" t="s">
-        <v>220</v>
-      </c>
-      <c r="C24" t="s">
-        <v>220</v>
-      </c>
-      <c r="D24" t="s">
-        <v>220</v>
-      </c>
-      <c r="E24" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>292</v>
-      </c>
-      <c r="B25" t="s">
-        <v>221</v>
-      </c>
-      <c r="C25" t="s">
-        <v>221</v>
-      </c>
-      <c r="D25" t="s">
-        <v>221</v>
-      </c>
-      <c r="E25" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>293</v>
-      </c>
-      <c r="B26" t="s">
-        <v>222</v>
-      </c>
-      <c r="C26" t="s">
-        <v>222</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="G29" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>296</v>
+      </c>
+      <c r="B30" t="s">
+        <v>225</v>
+      </c>
+      <c r="C30" t="s">
+        <v>225</v>
+      </c>
+      <c r="D30" t="s">
+        <v>225</v>
+      </c>
+      <c r="E30" t="s">
+        <v>225</v>
+      </c>
+      <c r="F30" t="s">
+        <v>346</v>
+      </c>
+      <c r="G30" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>297</v>
+      </c>
+      <c r="B31" t="s">
+        <v>226</v>
+      </c>
+      <c r="C31" t="s">
+        <v>226</v>
+      </c>
+      <c r="D31" t="s">
+        <v>226</v>
+      </c>
+      <c r="E31" t="s">
+        <v>226</v>
+      </c>
+      <c r="F31" t="s">
+        <v>346</v>
+      </c>
+      <c r="G31" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>298</v>
+      </c>
+      <c r="B32" t="s">
+        <v>232</v>
+      </c>
+      <c r="C32" t="s">
+        <v>227</v>
+      </c>
+      <c r="D32" t="s">
         <v>242</v>
       </c>
-      <c r="E26" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>294</v>
-      </c>
-      <c r="B27" t="s">
-        <v>223</v>
-      </c>
-      <c r="C27" t="s">
-        <v>223</v>
-      </c>
-      <c r="D27" t="s">
-        <v>223</v>
-      </c>
-      <c r="E27" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>295</v>
-      </c>
-      <c r="B28" t="s">
-        <v>224</v>
-      </c>
-      <c r="C28" t="s">
-        <v>224</v>
-      </c>
-      <c r="D28" t="s">
-        <v>224</v>
-      </c>
-      <c r="E28" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>296</v>
-      </c>
-      <c r="B29" t="s">
-        <v>225</v>
-      </c>
-      <c r="C29" t="s">
-        <v>225</v>
-      </c>
-      <c r="D29" t="s">
-        <v>225</v>
-      </c>
-      <c r="E29" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>297</v>
-      </c>
-      <c r="B30" t="s">
-        <v>226</v>
-      </c>
-      <c r="C30" t="s">
-        <v>226</v>
-      </c>
-      <c r="D30" t="s">
-        <v>226</v>
-      </c>
-      <c r="E30" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>298</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="E32" t="s">
         <v>227</v>
       </c>
-      <c r="C31" t="s">
-        <v>227</v>
-      </c>
-      <c r="D31" t="s">
-        <v>227</v>
-      </c>
-      <c r="E31" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="F32" t="s">
+        <v>344</v>
+      </c>
+      <c r="G32" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>299</v>
       </c>
-      <c r="B32" t="s">
-        <v>233</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="B33" t="s">
         <v>228</v>
       </c>
-      <c r="D32" t="s">
-        <v>243</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="C33" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="D33" t="s">
+        <v>228</v>
+      </c>
+      <c r="E33" t="s">
+        <v>228</v>
+      </c>
+      <c r="F33" t="s">
+        <v>366</v>
+      </c>
+      <c r="G33" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>300</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>229</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>229</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" t="s">
         <v>229</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E34" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="F34" t="s">
+        <v>229</v>
+      </c>
+      <c r="G34" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E35" s="5" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
+      <c r="F35" t="s">
+        <v>344</v>
+      </c>
+      <c r="G35" t="s">
+        <v>372</v>
+      </c>
+      <c r="N35" s="5"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B36" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C36" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D36" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="E36" s="6" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>232</v>
-      </c>
+      <c r="F36" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="N36" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:B2">
-    <sortState ref="A2:D35">
-      <sortCondition ref="A1:A35"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>